<commit_message>
Add damage reduction + increase enemies damage
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -371,7 +371,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,16 +414,16 @@
         <v>4.877057549928594</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>3</v>

</xml_diff>